<commit_message>
ui bdd+ddt registration: Done
</commit_message>
<xml_diff>
--- a/main/src/test/resources/xlsx/users.xlsx
+++ b/main/src/test/resources/xlsx/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oleksandr.c.BRILLIO\IdeaProjects\capstone-main\main\src\test\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1408EA-490A-4C58-920B-1A7A8BBB1611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE147958-D813-4F90-AC63-0F5717730AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="4005" windowWidth="28800" windowHeight="11325" xr2:uid="{992B54C3-16AE-4562-AD2E-95B9F3825C02}"/>
+    <workbookView xWindow="0" yWindow="4155" windowWidth="28800" windowHeight="11325" xr2:uid="{992B54C3-16AE-4562-AD2E-95B9F3825C02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>First Name</t>
   </si>
@@ -61,124 +61,127 @@
     <t>Jonson</t>
   </si>
   <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>1234567891</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. </t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>1/7/1990</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>One Inc.</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Sunnyvale</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>JohnJonson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs. </t>
+  </si>
+  <si>
+    <t>TomTomson</t>
+  </si>
+  <si>
+    <t>JackJackson</t>
+  </si>
+  <si>
+    <t>1/7/1991</t>
+  </si>
+  <si>
+    <t>1/7/1992</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Tomson</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Two Inc.</t>
+  </si>
+  <si>
+    <t>Three Inc.</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>Address 3</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>1234567892</t>
+  </si>
+  <si>
+    <t>1234567893</t>
+  </si>
+  <si>
+    <t>1111.0</t>
+  </si>
+  <si>
     <t>john_johnson@exaple.com</t>
   </si>
   <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>1234567891</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr. </t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>1/7/1990</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>One Inc.</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Zipcode</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Sunnyvale</t>
-  </si>
-  <si>
-    <t>User Name</t>
-  </si>
-  <si>
-    <t>JohnJonson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mrs. </t>
-  </si>
-  <si>
-    <t>TomTomson</t>
-  </si>
-  <si>
-    <t>JackJackson</t>
-  </si>
-  <si>
     <t>tom_tomson@exaple.com</t>
   </si>
   <si>
     <t>jack_jackson@exaple.com</t>
-  </si>
-  <si>
-    <t>1/7/1991</t>
-  </si>
-  <si>
-    <t>1/7/1992</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Tomson</t>
-  </si>
-  <si>
-    <t>Jackson</t>
-  </si>
-  <si>
-    <t>Two Inc.</t>
-  </si>
-  <si>
-    <t>Three Inc.</t>
-  </si>
-  <si>
-    <t>Address 1</t>
-  </si>
-  <si>
-    <t>Address 2</t>
-  </si>
-  <si>
-    <t>Address 3</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>Seattle</t>
-  </si>
-  <si>
-    <t>1234567892</t>
-  </si>
-  <si>
-    <t>1234567893</t>
   </si>
 </sst>
 </file>
@@ -231,8 +234,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -551,203 +554,210 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="17.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>1111</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N2">
+      <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="1">
         <v>94085</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>10</v>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3">
-        <v>1111</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3">
+      <c r="K3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1">
         <v>94085</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>46</v>
+      <c r="O3" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>1111</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4">
+      <c r="K4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="1">
         <v>94085</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>47</v>
+      <c r="O4" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -760,5 +770,8 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
+  <ignoredErrors>
+    <ignoredError sqref="O2:O4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
signup and login while checkout ui
</commit_message>
<xml_diff>
--- a/main/src/test/resources/xlsx/users.xlsx
+++ b/main/src/test/resources/xlsx/users.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oleksandr.c.BRILLIO\IdeaProjects\capstone-main\main\src\test\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1BCC70-A1FE-4281-AC56-4672FCCA73FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F96DE2-3931-458A-B449-8D7A20BC2CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4155" windowWidth="28800" windowHeight="11325" xr2:uid="{992B54C3-16AE-4562-AD2E-95B9F3825C02}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{992B54C3-16AE-4562-AD2E-95B9F3825C02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
   <si>
     <t>First Name</t>
   </si>
@@ -260,6 +261,69 @@
   </si>
   <si>
     <t>1234567896</t>
+  </si>
+  <si>
+    <t>CARD NUMBER</t>
+  </si>
+  <si>
+    <t>CVC</t>
+  </si>
+  <si>
+    <t>Expiration</t>
+  </si>
+  <si>
+    <t>4242 4242 4242 4242</t>
+  </si>
+  <si>
+    <t>4243 4242 4242 4242</t>
+  </si>
+  <si>
+    <t>4244 4242 4242 4242</t>
+  </si>
+  <si>
+    <t>4245 4242 4242 4242</t>
+  </si>
+  <si>
+    <t>4246 4242 4242 4242</t>
+  </si>
+  <si>
+    <t>4247 4242 4242 4242</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>12/2020</t>
+  </si>
+  <si>
+    <t>12/2021</t>
+  </si>
+  <si>
+    <t>12/2022</t>
+  </si>
+  <si>
+    <t>12/2023</t>
+  </si>
+  <si>
+    <t>12/2024</t>
+  </si>
+  <si>
+    <t>12/2025</t>
   </si>
 </sst>
 </file>
@@ -641,7 +705,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:O7"/>
+      <selection activeCell="R2" sqref="R2:R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,6 +769,15 @@
       <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -752,6 +825,15 @@
       <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="P2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -799,6 +881,15 @@
       <c r="O3" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="P3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -846,6 +937,15 @@
       <c r="O4" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="P4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -859,7 +959,7 @@
       </c>
       <c r="D5" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(S5:T5)</f>
-        <v>CMMM@exaple.com</v>
+        <v>TCPC@exaple.com</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>56</v>
@@ -894,9 +994,18 @@
       <c r="O5" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="P5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="S5" s="3" t="str">
         <f ca="1">CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65))</f>
-        <v>CMMM</v>
+        <v>TCPC</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>52</v>
@@ -914,7 +1023,7 @@
       </c>
       <c r="D6" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(S6,T5)</f>
-        <v>FBDR@exaple.com</v>
+        <v>FPTB@exaple.com</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>56</v>
@@ -949,9 +1058,18 @@
       <c r="O6" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="P6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="S6" s="3" t="str">
         <f ca="1">CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65))</f>
-        <v>FBDR</v>
+        <v>FPTB</v>
       </c>
       <c r="T6"/>
     </row>
@@ -967,7 +1085,7 @@
       </c>
       <c r="D7" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(S7,T5)</f>
-        <v>NLBK@exaple.com</v>
+        <v>JLIJ@exaple.com</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>56</v>
@@ -1002,9 +1120,18 @@
       <c r="O7" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="P7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="S7" s="3" t="str">
         <f ca="1">CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65))</f>
-        <v>NLBK</v>
+        <v>JLIJ</v>
       </c>
       <c r="T7"/>
     </row>

</xml_diff>

<commit_message>
pom test suit update
</commit_message>
<xml_diff>
--- a/main/src/test/resources/xlsx/users.xlsx
+++ b/main/src/test/resources/xlsx/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oleksandr.c.BRILLIO\IdeaProjects\capstone-main\main\src\test\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F96DE2-3931-458A-B449-8D7A20BC2CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BE0DB6-9C6B-48D5-B6ED-E484946E7BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{992B54C3-16AE-4562-AD2E-95B9F3825C02}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="92">
   <si>
     <t>First Name</t>
   </si>
@@ -171,18 +170,6 @@
   </si>
   <si>
     <t>1234567893</t>
-  </si>
-  <si>
-    <t>1111.0</t>
-  </si>
-  <si>
-    <t>john_johnson@exaple.com</t>
-  </si>
-  <si>
-    <t>tom_tomson@exaple.com</t>
-  </si>
-  <si>
-    <t>jack_jackson@exaple.com</t>
   </si>
   <si>
     <t>4</t>
@@ -330,18 +317,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -377,19 +356,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -705,7 +681,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R7"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,16 +746,16 @@
         <v>3</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -789,11 +765,12 @@
       <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>46</v>
+      <c r="D2" s="2" t="str">
+        <f ca="1">_xlfn.CONCAT(S2,T5)</f>
+        <v>DKCV@exaple.com</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
@@ -826,16 +803,20 @@
         <v>9</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
+      </c>
+      <c r="S2" s="3" t="str">
+        <f t="shared" ref="S2:S6" ca="1" si="0">CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65))</f>
+        <v>DKCV</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -845,11 +826,12 @@
       <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>47</v>
+      <c r="D3" s="2" t="str">
+        <f ca="1">_xlfn.CONCAT(S3,T5)</f>
+        <v>DCGT@exaple.com</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>28</v>
@@ -882,16 +864,20 @@
         <v>43</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="S3" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>DCGT</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -901,11 +887,12 @@
       <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>48</v>
+      <c r="D4" s="2" t="str">
+        <f ca="1">_xlfn.CONCAT(S4,T5)</f>
+        <v>XMOS@exaple.com</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>29</v>
@@ -938,46 +925,50 @@
         <v>44</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="S4" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>XMOS</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f ca="1">_xlfn.CONCAT(S5:T5)</f>
+        <v>GPSK@exaple.com</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(S5:T5)</f>
-        <v>TCPC@exaple.com</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>11</v>
@@ -992,56 +983,56 @@
         <v>94085</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="S5" s="3" t="str">
         <f ca="1">CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65))</f>
-        <v>TCPC</v>
+        <v>GPSK</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="4" t="str">
+        <v>57</v>
+      </c>
+      <c r="D6" s="2" t="str">
         <f ca="1">_xlfn.CONCAT(S6,T5)</f>
-        <v>FPTB@exaple.com</v>
+        <v>JRXN@exaple.com</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>39</v>
@@ -1056,54 +1047,53 @@
         <v>94085</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="S6" s="3" t="str">
-        <f ca="1">CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65))</f>
-        <v>FPTB</v>
-      </c>
-      <c r="T6"/>
+        <f t="shared" ca="1" si="0"/>
+        <v>JRXN</v>
+      </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="4" t="str">
+        <v>58</v>
+      </c>
+      <c r="D7" s="2" t="str">
         <f ca="1">_xlfn.CONCAT(S7,T5)</f>
-        <v>JLIJ@exaple.com</v>
+        <v>RAUN@exaple.com</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>40</v>
@@ -1118,33 +1108,26 @@
         <v>94085</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="S7" s="3" t="str">
         <f ca="1">CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65)) &amp; CHAR(INT(RAND()* 25 + 65))</f>
-        <v>JLIJ</v>
-      </c>
-      <c r="T7"/>
+        <v>RAUN</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{432C6E76-1AC1-4A59-BFC5-F5BAA27B8C24}"/>
-    <hyperlink ref="D3:D4" r:id="rId2" display="john_johnson@exaple.com" xr:uid="{27CAED58-F8BC-4011-A86D-B95D3D74B15B}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{3F6FA562-9ADE-405B-8E59-234789AD7F8D}"/>
-    <hyperlink ref="D4" r:id="rId4" xr:uid="{697929FB-108F-49E4-9209-08EF3F944EE7}"/>
-  </hyperlinks>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="O2:O4" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>